<commit_message>
Line graphs also work...
</commit_message>
<xml_diff>
--- a/acwef1/acwe2023.xlsx
+++ b/acwef1/acwe2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiel/devel/smallprograms/acwef1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DB985E-BD92-1143-B104-E3CD28D474DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEB773E-8E97-0B4B-AF17-617E20292D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{12AA6836-9E2D-4D41-8070-357FB3F2415B}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,10 +590,10 @@
         <v>25</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -616,7 +616,7 @@
         <v>18</v>
       </c>
       <c r="G3">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>18</v>
@@ -642,10 +642,10 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -694,7 +694,7 @@
         <v>6</v>
       </c>
       <c r="G6">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H6">
         <v>6</v>

</xml_diff>

<commit_message>
Updated settings, all plots complete now.
</commit_message>
<xml_diff>
--- a/acwef1/acwe2023.xlsx
+++ b/acwef1/acwe2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiel/devel/smallprograms/acwef1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEB773E-8E97-0B4B-AF17-617E20292D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A67D153-28AF-7449-8E7C-AA1F75494349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{12AA6836-9E2D-4D41-8070-357FB3F2415B}"/>
+    <workbookView xWindow="2220" yWindow="1920" windowWidth="26580" windowHeight="12880" xr2:uid="{12AA6836-9E2D-4D41-8070-357FB3F2415B}"/>
   </bookViews>
   <sheets>
     <sheet name="Coureurs" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>Max Verstappen</t>
   </si>
@@ -180,6 +180,63 @@
   </si>
   <si>
     <t>Australië</t>
+  </si>
+  <si>
+    <t>Casper</t>
+  </si>
+  <si>
+    <t>Raymond</t>
+  </si>
+  <si>
+    <t>Niels</t>
+  </si>
+  <si>
+    <t>Erik</t>
+  </si>
+  <si>
+    <t>Grietje</t>
+  </si>
+  <si>
+    <t>Arjan T.</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Michiel</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Rodi</t>
+  </si>
+  <si>
+    <t>Arjan Z.</t>
+  </si>
+  <si>
+    <t>Hans</t>
+  </si>
+  <si>
+    <t>Kitty</t>
+  </si>
+  <si>
+    <t>Stan</t>
+  </si>
+  <si>
+    <t>Erwin</t>
+  </si>
+  <si>
+    <t>Mees</t>
+  </si>
+  <si>
+    <t>Jordi</t>
+  </si>
+  <si>
+    <t>Wietse</t>
+  </si>
+  <si>
+    <t>Isolde</t>
   </si>
 </sst>
 </file>
@@ -534,7 +591,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G2" sqref="G2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,10 +647,10 @@
         <v>25</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -616,10 +673,10 @@
         <v>18</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="H3">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -642,10 +699,10 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -671,7 +728,7 @@
         <v>12</v>
       </c>
       <c r="H5">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -694,10 +751,10 @@
         <v>6</v>
       </c>
       <c r="G6">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -723,7 +780,7 @@
         <v>10</v>
       </c>
       <c r="H7">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -775,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -853,7 +910,7 @@
         <v>4</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -905,7 +962,7 @@
         <v>8</v>
       </c>
       <c r="H14">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -931,7 +988,7 @@
         <v>15</v>
       </c>
       <c r="H15">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1061,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1306,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF36770-6B00-FF44-A9D9-DC44E7FE0BCE}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,6 +1451,386 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>7</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Figures now ordered alphabetically.
</commit_message>
<xml_diff>
--- a/acwef1/acwe2023.xlsx
+++ b/acwef1/acwe2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiel/devel/smallprograms/acwef1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A67D153-28AF-7449-8E7C-AA1F75494349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC69716-B3F1-5F4F-BAC4-FC2542128EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="1920" windowWidth="26580" windowHeight="12880" xr2:uid="{12AA6836-9E2D-4D41-8070-357FB3F2415B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
   <si>
     <t>Max Verstappen</t>
   </si>
@@ -237,6 +237,66 @@
   </si>
   <si>
     <t>Isolde</t>
+  </si>
+  <si>
+    <t>Azerbeidzjan</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Emilia-Romagna</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Spanje</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Oostenrijk</t>
+  </si>
+  <si>
+    <t>Groot-Brittanië</t>
+  </si>
+  <si>
+    <t>Hongarije</t>
+  </si>
+  <si>
+    <t>België</t>
+  </si>
+  <si>
+    <t>Nederland</t>
+  </si>
+  <si>
+    <t>Italië</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Verenigde Staten</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Brazilië</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Abu Dhabi</t>
   </si>
 </sst>
 </file>
@@ -588,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DCEF33-6C52-9C4D-82E6-A5321B9B8DD1}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,7 +661,7 @@
     <col min="7" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -626,8 +686,68 @@
       <c r="H1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T1" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" t="s">
+        <v>78</v>
+      </c>
+      <c r="V1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -647,13 +767,73 @@
         <v>25</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -673,13 +853,73 @@
         <v>18</v>
       </c>
       <c r="G3">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -704,8 +944,68 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -725,13 +1025,73 @@
         <v>12</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -751,13 +1111,73 @@
         <v>6</v>
       </c>
       <c r="G6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -777,13 +1197,73 @@
         <v>10</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -808,8 +1288,68 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -829,13 +1369,73 @@
         <v>2</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -860,8 +1460,68 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -886,8 +1546,68 @@
       <c r="H11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -907,13 +1627,73 @@
         <v>4</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -938,8 +1718,68 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -959,13 +1799,73 @@
         <v>8</v>
       </c>
       <c r="G14">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -985,13 +1885,73 @@
         <v>15</v>
       </c>
       <c r="G15">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1016,8 +1976,68 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1042,8 +2062,68 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1068,8 +2148,68 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1094,8 +2234,68 @@
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1115,13 +2315,73 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1144,6 +2404,66 @@
         <v>0</v>
       </c>
       <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Most recent results and page proof figures.
</commit_message>
<xml_diff>
--- a/acwef1/acwe2023.xlsx
+++ b/acwef1/acwe2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiel/devel/smallprograms/acwef1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC69716-B3F1-5F4F-BAC4-FC2542128EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757811B9-FCA4-B848-A7E1-9A3413DB91F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="1920" windowWidth="26580" windowHeight="12880" xr2:uid="{12AA6836-9E2D-4D41-8070-357FB3F2415B}"/>
+    <workbookView xWindow="11000" yWindow="2160" windowWidth="17800" windowHeight="13460" xr2:uid="{12AA6836-9E2D-4D41-8070-357FB3F2415B}"/>
   </bookViews>
   <sheets>
     <sheet name="Coureurs" sheetId="1" r:id="rId1"/>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DCEF33-6C52-9C4D-82E6-A5321B9B8DD1}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,7 +767,7 @@
         <v>25</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -853,7 +853,7 @@
         <v>18</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -939,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1025,7 +1025,7 @@
         <v>12</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1111,7 +1111,7 @@
         <v>6</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1197,7 +1197,7 @@
         <v>10</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1369,7 +1369,7 @@
         <v>2</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1885,7 +1885,7 @@
         <v>15</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1971,7 +1971,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>0</v>

</xml_diff>

<commit_message>
Updated score with Australia.
</commit_message>
<xml_diff>
--- a/acwef1/acwe2023.xlsx
+++ b/acwef1/acwe2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiel/devel/smallprograms/acwef1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757811B9-FCA4-B848-A7E1-9A3413DB91F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D8AC1E-9B7D-9A43-BA3A-8DA94277E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11000" yWindow="2160" windowWidth="17800" windowHeight="13460" xr2:uid="{12AA6836-9E2D-4D41-8070-357FB3F2415B}"/>
+    <workbookView xWindow="2160" yWindow="1580" windowWidth="24120" windowHeight="13620" xr2:uid="{12AA6836-9E2D-4D41-8070-357FB3F2415B}"/>
   </bookViews>
   <sheets>
     <sheet name="Coureurs" sheetId="1" r:id="rId1"/>
@@ -651,7 +651,7 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -770,7 +770,7 @@
         <v>19</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -856,7 +856,7 @@
         <v>25</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1200,7 +1200,7 @@
         <v>10</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1716,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1888,7 +1888,7 @@
         <v>15</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -2060,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2232,7 +2232,7 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <v>0</v>

</xml_diff>